<commit_message>
Testing with real data
</commit_message>
<xml_diff>
--- a/data/new/REAL.xlsx
+++ b/data/new/REAL.xlsx
@@ -9,12 +9,15 @@
   <sheets>
     <sheet r:id="rId1" sheetId="1" name="REAL"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0">REAL!$A$1:$X$1</definedName>
+  </definedNames>
   <calcPr fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="65">
   <si>
     <t>Sociedad</t>
   </si>
@@ -86,6 +89,129 @@
   </si>
   <si>
     <t>Observaciones</t>
+  </si>
+  <si>
+    <t>E001</t>
+  </si>
+  <si>
+    <t>100000002602</t>
+  </si>
+  <si>
+    <t>E001 - INVERSION APLICACIONES I&amp;C</t>
+  </si>
+  <si>
+    <t>Servicios informáticos</t>
+  </si>
+  <si>
+    <t>24.12.2022</t>
+  </si>
+  <si>
+    <t>UN</t>
+  </si>
+  <si>
+    <t>Hito 5: Fin del soporte post arranque</t>
+  </si>
+  <si>
+    <t>WE</t>
+  </si>
+  <si>
+    <t>PRJ0032035-SptePostArra</t>
+  </si>
+  <si>
+    <t>ibernal</t>
+  </si>
+  <si>
+    <t>EN00667</t>
+  </si>
+  <si>
+    <t>100000002607</t>
+  </si>
+  <si>
+    <t>E001 - INVERSION APLICACIONES COMPRAS</t>
+  </si>
+  <si>
+    <t>Perfil_Senior Funcional_ERP (€/h)</t>
+  </si>
+  <si>
+    <t>PRJ0032270-Fin</t>
+  </si>
+  <si>
+    <t>EN00338</t>
+  </si>
+  <si>
+    <t>100000002606</t>
+  </si>
+  <si>
+    <t>E001 - INVERSION APLICACIONES PRODUCCION</t>
+  </si>
+  <si>
+    <t>DMND5713,6882,7943-Fin</t>
+  </si>
+  <si>
+    <t>EN00521</t>
+  </si>
+  <si>
+    <t>EN00694</t>
+  </si>
+  <si>
+    <t>EN00540</t>
+  </si>
+  <si>
+    <t>PRJ0032270-Fin2de2</t>
+  </si>
+  <si>
+    <t>€/Jornada Técnico IT</t>
+  </si>
+  <si>
+    <t>EvoSO99-22-2de2</t>
+  </si>
+  <si>
+    <t>EN00110</t>
+  </si>
+  <si>
+    <t>100000002600</t>
+  </si>
+  <si>
+    <t>E001 - IT INVERSION APLICACIONES</t>
+  </si>
+  <si>
+    <t>€/hora Desarrollo Evolutivo y Proyectos</t>
+  </si>
+  <si>
+    <t>PRJ0032438-MotorIngestas</t>
+  </si>
+  <si>
+    <t>EN00720</t>
+  </si>
+  <si>
+    <t>100000002124</t>
+  </si>
+  <si>
+    <t>E001-TRANSFORMACION DIGITAL IT</t>
+  </si>
+  <si>
+    <t>ENTD_TD003</t>
+  </si>
+  <si>
+    <t>EV01</t>
+  </si>
+  <si>
+    <t>ES/2-V/1216/E.03.14</t>
+  </si>
+  <si>
+    <t>Comercialización Acciona Green</t>
+  </si>
+  <si>
+    <t>CRM365-GoLiveNov (FdS)</t>
+  </si>
+  <si>
+    <t>EN00634</t>
+  </si>
+  <si>
+    <t>36,280-</t>
+  </si>
+  <si>
+    <t>CRM365-GoLive-FdS-Nov</t>
   </si>
 </sst>
 </file>
@@ -93,7 +219,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -102,23 +228,31 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="9"/>
       <color rgb="FFffffff"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FFffffff"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF000000"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -153,15 +287,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="26">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="49" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="1" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="1" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
@@ -179,22 +316,52 @@
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="49" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="1" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="1" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="49" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="1" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="1" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -499,41 +666,39 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:X1"/>
+  <dimension ref="A1:X14"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1">
-      <pane state="frozen" activePane="bottomLeft" topLeftCell="A2" ySplit="1" xSplit="0"/>
-    </sheetView>
+    <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="10" width="7.2907142857142855" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="11" width="18.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="10" width="37.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="12" width="9.290714285714287" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="13" width="17.005" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="12" width="6.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="12" width="6.862142857142857" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="12" width="6.2907142857142855" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="10" width="34.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="10" width="11.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="10" width="11.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="14" width="9.290714285714287" customWidth="1" bestFit="1"/>
-    <col min="13" max="13" style="10" width="6.005" customWidth="1" bestFit="1"/>
-    <col min="14" max="14" style="10" width="43.86214285714286" customWidth="1" bestFit="1"/>
-    <col min="15" max="15" style="14" width="11.290714285714287" customWidth="1" bestFit="1"/>
-    <col min="16" max="16" style="10" width="5.433571428571429" customWidth="1" bestFit="1"/>
-    <col min="17" max="17" style="12" width="14.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="18" max="18" style="10" width="37.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="19" max="19" style="10" width="27.862142857142857" customWidth="1" bestFit="1"/>
-    <col min="20" max="20" style="10" width="25.862142857142857" customWidth="1" bestFit="1"/>
-    <col min="21" max="21" style="10" width="11.005" customWidth="1" bestFit="1"/>
-    <col min="22" max="22" style="12" width="15.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="23" max="23" style="10" width="11.290714285714287" customWidth="1" bestFit="1"/>
-    <col min="24" max="24" style="10" width="37.005" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="19" width="7.2907142857142855" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="20" width="18.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="21" width="37.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="22" width="12.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="23" width="11.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="22" width="6.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="22" width="6.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="22" width="6.2907142857142855" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="21" width="34.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="19" width="11.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="19" width="11.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="24" width="9.290714285714287" customWidth="1" bestFit="1"/>
+    <col min="13" max="13" style="25" width="6.005" customWidth="1" bestFit="1"/>
+    <col min="14" max="14" style="21" width="43.86214285714286" customWidth="1" bestFit="1"/>
+    <col min="15" max="15" style="24" width="11.290714285714287" customWidth="1" bestFit="1"/>
+    <col min="16" max="16" style="19" width="5.433571428571429" customWidth="1" bestFit="1"/>
+    <col min="17" max="17" style="22" width="11.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="18" max="18" style="21" width="37.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="19" max="19" style="21" width="27.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="20" max="20" style="19" width="25.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="21" max="21" style="19" width="11.005" customWidth="1" bestFit="1"/>
+    <col min="22" max="22" style="22" width="12.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="23" max="23" style="19" width="11.290714285714287" customWidth="1" bestFit="1"/>
+    <col min="24" max="24" style="19" width="37.005" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="37.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -543,19 +708,19 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
@@ -567,45 +732,955 @@
       <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="L1" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="M1" s="6" t="s">
         <v>12</v>
       </c>
       <c r="N1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="6" t="s">
+      <c r="O1" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="7" t="s">
+      <c r="P1" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="Q1" s="3" t="s">
         <v>16</v>
       </c>
       <c r="R1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="8" t="s">
+      <c r="S1" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="T1" s="10" t="s">
         <v>19</v>
       </c>
       <c r="U1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="2" t="s">
+      <c r="V1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="9" t="s">
+      <c r="W1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="9" t="s">
+      <c r="X1" s="1" t="s">
         <v>23</v>
       </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+      <c r="A2" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" s="14">
+        <v>10000452</v>
+      </c>
+      <c r="E2" s="15">
+        <v>3101307952</v>
+      </c>
+      <c r="F2" s="14">
+        <v>50</v>
+      </c>
+      <c r="G2" s="14">
+        <v>2022</v>
+      </c>
+      <c r="H2" s="14">
+        <v>12</v>
+      </c>
+      <c r="I2" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="J2" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="K2" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="L2" s="16">
+        <v>1</v>
+      </c>
+      <c r="M2" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="N2" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="O2" s="16">
+        <v>11840</v>
+      </c>
+      <c r="P2" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q2" s="14">
+        <v>5001653451</v>
+      </c>
+      <c r="R2" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="S2" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="T2" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="U2" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="V2" s="14">
+        <v>1005434489</v>
+      </c>
+      <c r="W2" s="18"/>
+      <c r="X2" s="18"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+      <c r="A3" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="D3" s="14">
+        <v>10000426</v>
+      </c>
+      <c r="E3" s="15">
+        <v>3101416843</v>
+      </c>
+      <c r="F3" s="14">
+        <v>90</v>
+      </c>
+      <c r="G3" s="14">
+        <v>2022</v>
+      </c>
+      <c r="H3" s="14">
+        <v>12</v>
+      </c>
+      <c r="I3" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="J3" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="K3" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="L3" s="16">
+        <v>45.4</v>
+      </c>
+      <c r="M3" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="N3" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="O3" s="16">
+        <v>3304.21</v>
+      </c>
+      <c r="P3" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q3" s="14">
+        <v>5001653472</v>
+      </c>
+      <c r="R3" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="S3" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="T3" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="U3" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="V3" s="14">
+        <v>1005434490</v>
+      </c>
+      <c r="W3" s="18"/>
+      <c r="X3" s="18"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+      <c r="A4" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="D4" s="14">
+        <v>10000426</v>
+      </c>
+      <c r="E4" s="15">
+        <v>3101418059</v>
+      </c>
+      <c r="F4" s="14">
+        <v>20</v>
+      </c>
+      <c r="G4" s="14">
+        <v>2022</v>
+      </c>
+      <c r="H4" s="14">
+        <v>12</v>
+      </c>
+      <c r="I4" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="J4" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="K4" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="L4" s="16">
+        <v>170.2</v>
+      </c>
+      <c r="M4" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="N4" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="O4" s="16">
+        <v>12387.16</v>
+      </c>
+      <c r="P4" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q4" s="14">
+        <v>5001653473</v>
+      </c>
+      <c r="R4" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="S4" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="T4" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="U4" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="V4" s="14">
+        <v>1005434491</v>
+      </c>
+      <c r="W4" s="18"/>
+      <c r="X4" s="18"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+      <c r="A5" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="D5" s="14">
+        <v>10000426</v>
+      </c>
+      <c r="E5" s="15">
+        <v>3101418059</v>
+      </c>
+      <c r="F5" s="14">
+        <v>40</v>
+      </c>
+      <c r="G5" s="14">
+        <v>2022</v>
+      </c>
+      <c r="H5" s="14">
+        <v>12</v>
+      </c>
+      <c r="I5" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="J5" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="K5" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="L5" s="16">
+        <v>102.51</v>
+      </c>
+      <c r="M5" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="N5" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="O5" s="16">
+        <v>7460.68</v>
+      </c>
+      <c r="P5" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q5" s="14">
+        <v>5001653473</v>
+      </c>
+      <c r="R5" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="S5" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="T5" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="U5" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="V5" s="14">
+        <v>1005434491</v>
+      </c>
+      <c r="W5" s="18"/>
+      <c r="X5" s="18"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+      <c r="A6" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="D6" s="14">
+        <v>10000426</v>
+      </c>
+      <c r="E6" s="15">
+        <v>3101418059</v>
+      </c>
+      <c r="F6" s="14">
+        <v>50</v>
+      </c>
+      <c r="G6" s="14">
+        <v>2022</v>
+      </c>
+      <c r="H6" s="14">
+        <v>12</v>
+      </c>
+      <c r="I6" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="J6" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="K6" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="L6" s="16">
+        <v>34.63</v>
+      </c>
+      <c r="M6" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="N6" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="O6" s="16">
+        <v>2520.37</v>
+      </c>
+      <c r="P6" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q6" s="14">
+        <v>5001653473</v>
+      </c>
+      <c r="R6" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="S6" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="T6" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="U6" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="V6" s="14">
+        <v>1005434491</v>
+      </c>
+      <c r="W6" s="18"/>
+      <c r="X6" s="18"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
+      <c r="A7" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="D7" s="14">
+        <v>10000426</v>
+      </c>
+      <c r="E7" s="15">
+        <v>3101416842</v>
+      </c>
+      <c r="F7" s="14">
+        <v>10</v>
+      </c>
+      <c r="G7" s="14">
+        <v>2022</v>
+      </c>
+      <c r="H7" s="14">
+        <v>12</v>
+      </c>
+      <c r="I7" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="J7" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="K7" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="L7" s="16">
+        <v>47.93</v>
+      </c>
+      <c r="M7" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="N7" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="O7" s="16">
+        <v>3488.35</v>
+      </c>
+      <c r="P7" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q7" s="14">
+        <v>5001653474</v>
+      </c>
+      <c r="R7" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="S7" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="T7" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="U7" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="V7" s="14">
+        <v>1005434492</v>
+      </c>
+      <c r="W7" s="18"/>
+      <c r="X7" s="18"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
+      <c r="A8" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="D8" s="14">
+        <v>10075367</v>
+      </c>
+      <c r="E8" s="15">
+        <v>3101432168</v>
+      </c>
+      <c r="F8" s="14">
+        <v>10</v>
+      </c>
+      <c r="G8" s="14">
+        <v>2022</v>
+      </c>
+      <c r="H8" s="14">
+        <v>12</v>
+      </c>
+      <c r="I8" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="J8" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="K8" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="L8" s="16">
+        <v>1</v>
+      </c>
+      <c r="M8" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="N8" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="O8" s="16">
+        <v>777</v>
+      </c>
+      <c r="P8" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q8" s="14">
+        <v>5001653463</v>
+      </c>
+      <c r="R8" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="S8" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="T8" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="U8" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="V8" s="14">
+        <v>1005434630</v>
+      </c>
+      <c r="W8" s="18"/>
+      <c r="X8" s="18"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
+      <c r="A9" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="D9" s="14">
+        <v>10048866</v>
+      </c>
+      <c r="E9" s="15">
+        <v>3101434312</v>
+      </c>
+      <c r="F9" s="14">
+        <v>10</v>
+      </c>
+      <c r="G9" s="14">
+        <v>2022</v>
+      </c>
+      <c r="H9" s="14">
+        <v>12</v>
+      </c>
+      <c r="I9" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="J9" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="K9" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="L9" s="16">
+        <v>391</v>
+      </c>
+      <c r="M9" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="N9" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="O9" s="16">
+        <v>21802.16</v>
+      </c>
+      <c r="P9" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q9" s="14">
+        <v>5001653467</v>
+      </c>
+      <c r="R9" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="S9" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="T9" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="U9" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="V9" s="14">
+        <v>1005434634</v>
+      </c>
+      <c r="W9" s="18"/>
+      <c r="X9" s="18"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
+      <c r="A10" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="D10" s="14">
+        <v>10048866</v>
+      </c>
+      <c r="E10" s="15">
+        <v>3101434312</v>
+      </c>
+      <c r="F10" s="14">
+        <v>10</v>
+      </c>
+      <c r="G10" s="14">
+        <v>2022</v>
+      </c>
+      <c r="H10" s="14">
+        <v>12</v>
+      </c>
+      <c r="I10" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="J10" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="K10" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="L10" s="16">
+        <v>391</v>
+      </c>
+      <c r="M10" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="N10" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="O10" s="16">
+        <v>21802.16</v>
+      </c>
+      <c r="P10" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q10" s="14">
+        <v>5001653467</v>
+      </c>
+      <c r="R10" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="S10" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="T10" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="U10" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="V10" s="14">
+        <v>1005434634</v>
+      </c>
+      <c r="W10" s="18"/>
+      <c r="X10" s="18"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
+      <c r="A11" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="C11" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="D11" s="14">
+        <v>10048866</v>
+      </c>
+      <c r="E11" s="15">
+        <v>3101433528</v>
+      </c>
+      <c r="F11" s="14">
+        <v>10</v>
+      </c>
+      <c r="G11" s="14">
+        <v>2022</v>
+      </c>
+      <c r="H11" s="14">
+        <v>12</v>
+      </c>
+      <c r="I11" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="J11" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="K11" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="L11" s="16">
+        <v>196.75</v>
+      </c>
+      <c r="M11" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="N11" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="O11" s="16">
+        <v>10970.78</v>
+      </c>
+      <c r="P11" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q11" s="14">
+        <v>5001653464</v>
+      </c>
+      <c r="R11" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="S11" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="T11" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="U11" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="V11" s="14">
+        <v>1005434631</v>
+      </c>
+      <c r="W11" s="18"/>
+      <c r="X11" s="18"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
+      <c r="A12" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="B12" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="C12" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="D12" s="14">
+        <v>10048866</v>
+      </c>
+      <c r="E12" s="15">
+        <v>3101433528</v>
+      </c>
+      <c r="F12" s="14">
+        <v>20</v>
+      </c>
+      <c r="G12" s="14">
+        <v>2022</v>
+      </c>
+      <c r="H12" s="14">
+        <v>12</v>
+      </c>
+      <c r="I12" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="J12" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="K12" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="L12" s="16">
+        <v>36.28</v>
+      </c>
+      <c r="M12" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="N12" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="O12" s="16">
+        <v>2022.97</v>
+      </c>
+      <c r="P12" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q12" s="14">
+        <v>5001653464</v>
+      </c>
+      <c r="R12" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="S12" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="T12" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="U12" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="V12" s="14">
+        <v>1005434631</v>
+      </c>
+      <c r="W12" s="18"/>
+      <c r="X12" s="18"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
+      <c r="A13" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="D13" s="14">
+        <v>10048866</v>
+      </c>
+      <c r="E13" s="15">
+        <v>3101433528</v>
+      </c>
+      <c r="F13" s="14">
+        <v>20</v>
+      </c>
+      <c r="G13" s="14">
+        <v>2022</v>
+      </c>
+      <c r="H13" s="14">
+        <v>12</v>
+      </c>
+      <c r="I13" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="J13" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="K13" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="L13" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="M13" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="N13" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="O13" s="16">
+        <v>-2022.97</v>
+      </c>
+      <c r="P13" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q13" s="14">
+        <v>5001653465</v>
+      </c>
+      <c r="R13" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="S13" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="T13" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="U13" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="V13" s="14">
+        <v>1005434632</v>
+      </c>
+      <c r="W13" s="18"/>
+      <c r="X13" s="18"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
+      <c r="A14" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="B14" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="C14" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="D14" s="14">
+        <v>10048866</v>
+      </c>
+      <c r="E14" s="15">
+        <v>3101433528</v>
+      </c>
+      <c r="F14" s="14">
+        <v>20</v>
+      </c>
+      <c r="G14" s="14">
+        <v>2022</v>
+      </c>
+      <c r="H14" s="14">
+        <v>12</v>
+      </c>
+      <c r="I14" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="J14" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="K14" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="L14" s="16">
+        <v>36.82</v>
+      </c>
+      <c r="M14" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="N14" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="O14" s="16">
+        <v>2053.08</v>
+      </c>
+      <c r="P14" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q14" s="14">
+        <v>5001653466</v>
+      </c>
+      <c r="R14" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="S14" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="T14" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="U14" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="V14" s="14">
+        <v>1005434633</v>
+      </c>
+      <c r="W14" s="18"/>
+      <c r="X14" s="18"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>